<commit_message>
Extend Search function's deadline
</commit_message>
<xml_diff>
--- a/Plan-QuanLyThuVien-QuocBinh-HoangHuan.xlsx
+++ b/Plan-QuanLyThuVien-QuocBinh-HoangHuan.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\2.PTUD\QuanLyThuVien\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" tabRatio="500"/>
   </bookViews>
@@ -13,7 +18,7 @@
     <sheet name="Communication Plan" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -275,7 +280,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="m/d;@"/>
@@ -572,7 +577,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -704,7 +709,7 @@
                   <c:v>42648</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42642</c:v>
+                  <c:v>42649</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>42650</c:v>
@@ -727,7 +732,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
             </c:ext>
@@ -757,7 +762,7 @@
                 <a:srgbClr val="0000FF"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -772,7 +777,7 @@
                 <a:srgbClr val="0000FF"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -787,7 +792,7 @@
                 <a:srgbClr val="008000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000006-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -802,7 +807,7 @@
                 <a:srgbClr val="008000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000008-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -817,7 +822,7 @@
                 <a:srgbClr val="008000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000A-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -832,7 +837,7 @@
                 <a:srgbClr val="008000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000C-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -847,7 +852,7 @@
                 <a:srgbClr val="008000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000E-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -862,7 +867,7 @@
                 <a:srgbClr val="008000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000010-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -877,7 +882,7 @@
                 <a:srgbClr val="008000"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000012-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -892,7 +897,7 @@
                 <a:srgbClr val="FF6600"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000014-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -907,7 +912,7 @@
                 <a:srgbClr val="FF6600"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000016-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -922,7 +927,7 @@
                 <a:srgbClr val="FF6600"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000018-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -937,7 +942,7 @@
                 <a:srgbClr val="FF6600"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001A-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -952,7 +957,7 @@
                 <a:srgbClr val="FF6600"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001C-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -967,7 +972,7 @@
                 <a:srgbClr val="660066"/>
               </a:solidFill>
             </c:spPr>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000001E-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
               </c:ext>
@@ -1054,7 +1059,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>3</c:v>
@@ -1086,7 +1091,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000001F-8D9F-4A7B-AA73-B2B28EF7DCAB}"/>
             </c:ext>
@@ -1512,8 +1517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1752,14 +1757,14 @@
         <v>42645</v>
       </c>
       <c r="D18" s="7">
-        <v>42647</v>
+        <v>42648</v>
       </c>
       <c r="E18" s="3">
         <f>D18-C18</f>
-        <v>2</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>14</v>
+        <v>3</v>
+      </c>
+      <c r="F18" s="31" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="21.95" customHeight="1">
@@ -1812,10 +1817,10 @@
         <v>79</v>
       </c>
       <c r="C21" s="7">
-        <v>42642</v>
+        <v>42649</v>
       </c>
       <c r="D21" s="7">
-        <v>42644</v>
+        <v>42651</v>
       </c>
       <c r="E21" s="3">
         <f t="shared" si="0"/>

</xml_diff>